<commit_message>
Updates to schema: multiple contributor roles, misc tidying
</commit_message>
<xml_diff>
--- a/schema/excel/metadata.xlsx
+++ b/schema/excel/metadata.xlsx
@@ -456,7 +456,7 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>contributor__contributor_role</t>
+          <t>contributor__contributor_roles</t>
         </is>
       </c>
     </row>
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,7 +482,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>dataset__title</t>
+          <t>dataset__titles</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -492,20 +492,25 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>dataset__submission_date</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>dataset__access_date</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>dataset__contributors</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>dataset__resolvable_persistent_identifiers</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>dataset__funding_references</t>
         </is>
@@ -645,7 +650,7 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>contributor__contributor_role</t>
+          <t>contributor__contributor_roles</t>
         </is>
       </c>
     </row>
@@ -660,7 +665,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -671,7 +676,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>dataset__title</t>
+          <t>dataset__titles</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -681,20 +686,25 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>dataset__submission_date</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>dataset__access_date</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>dataset__contributors</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>dataset__resolvable_persistent_identifiers</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>dataset__funding_references</t>
         </is>

</xml_diff>